<commit_message>
feat(tarifas): implementar fluxo inicial de processamento de tarifas bancárias
- adiciona ProcessadorTarifas com integração a RepositorioParametros e RepositorioContasBancarias
- leitura da planilha de tarifas via LeitorTarifas
- salva conta de tarifas bancárias e vincula contas correntes a contas contábeis
- pendente: ajuste no LeitorTarifas para ignorar linhas em branco/somatório
</commit_message>
<xml_diff>
--- a/data/input/MODELO DE PLANILHA.xlsx
+++ b/data/input/MODELO DE PLANILHA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\001 - MODELO\001 - PORTIFÓLIO\006 - projetos\conversor-planilha-txt-dominio\data\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\OneDrive\Documentos\014 - PORTIFOLIO\conversor-planilha-txt-dominio\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC995C4A-80D5-4566-B0A5-6DD4997B409E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B16BCEF-47C3-4559-A281-66FB7AC80823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="843" activeTab="4" xr2:uid="{DDA27094-FF0A-42D4-8366-22E4AF05EBD8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="843" activeTab="1" xr2:uid="{DDA27094-FF0A-42D4-8366-22E4AF05EBD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Contas pagas" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
   <si>
     <t>EMPRESA</t>
   </si>
@@ -134,6 +134,27 @@
   </si>
   <si>
     <t>DOCUMENTO</t>
+  </si>
+  <si>
+    <t>GRUPO XYZ</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>4567-8</t>
+  </si>
+  <si>
+    <t>TARIFA - BB</t>
+  </si>
+  <si>
+    <t>BRADESCO</t>
+  </si>
+  <si>
+    <t>8765-4</t>
+  </si>
+  <si>
+    <t>TARIFA - BRADESCO</t>
   </si>
 </sst>
 </file>
@@ -967,18 +988,18 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="77.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23" style="46" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" style="51" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" style="51" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1001,7 +1022,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
@@ -1011,7 +1032,7 @@
       <c r="G2" s="49"/>
       <c r="H2" s="47"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
@@ -1021,7 +1042,7 @@
       <c r="G3" s="49"/>
       <c r="H3" s="47"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
@@ -1031,7 +1052,7 @@
       <c r="G4" s="49"/>
       <c r="H4" s="47"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
@@ -1041,7 +1062,7 @@
       <c r="G5" s="49"/>
       <c r="H5" s="47"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
@@ -1051,7 +1072,7 @@
       <c r="G6" s="49"/>
       <c r="H6" s="47"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
@@ -1061,7 +1082,7 @@
       <c r="G7" s="49"/>
       <c r="H7" s="47"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
@@ -1070,7 +1091,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="49"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
@@ -1079,7 +1100,7 @@
       <c r="F9" s="4"/>
       <c r="G9" s="49"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
@@ -1088,7 +1109,7 @@
       <c r="F10" s="4"/>
       <c r="G10" s="49"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
@@ -1097,7 +1118,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="49"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
@@ -1106,7 +1127,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="49"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
@@ -1115,7 +1136,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="49"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
@@ -1124,7 +1145,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="49"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
@@ -1133,7 +1154,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="49"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
@@ -1142,7 +1163,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="49"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
@@ -1151,7 +1172,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="49"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
@@ -1160,7 +1181,7 @@
       <c r="F18" s="4"/>
       <c r="G18" s="49"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
@@ -1169,7 +1190,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="49"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
@@ -1178,7 +1199,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="49"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
@@ -1187,7 +1208,7 @@
       <c r="F21" s="4"/>
       <c r="G21" s="49"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
@@ -1196,7 +1217,7 @@
       <c r="F22" s="4"/>
       <c r="G22" s="49"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
@@ -1205,7 +1226,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="49"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
@@ -1214,7 +1235,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="49"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="3"/>
       <c r="C25" s="4"/>
@@ -1223,7 +1244,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="49"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="3"/>
       <c r="C26" s="4"/>
@@ -1232,7 +1253,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="49"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="3"/>
       <c r="C27" s="4"/>
@@ -1241,7 +1262,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="49"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="3"/>
       <c r="C28" s="4"/>
@@ -1250,7 +1271,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="49"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="3"/>
       <c r="C29" s="4"/>
@@ -1259,7 +1280,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="49"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="3"/>
       <c r="C30" s="4"/>
@@ -1268,7 +1289,7 @@
       <c r="F30" s="4"/>
       <c r="G30" s="49"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="3"/>
       <c r="C31" s="4"/>
@@ -1277,7 +1298,7 @@
       <c r="F31" s="4"/>
       <c r="G31" s="49"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="3"/>
       <c r="C32" s="4"/>
@@ -1286,7 +1307,7 @@
       <c r="F32" s="4"/>
       <c r="G32" s="49"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="3"/>
       <c r="C33" s="4"/>
@@ -1295,7 +1316,7 @@
       <c r="F33" s="4"/>
       <c r="G33" s="49"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="3"/>
       <c r="C34" s="4"/>
@@ -1304,7 +1325,7 @@
       <c r="F34" s="4"/>
       <c r="G34" s="49"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="3"/>
       <c r="C35" s="4"/>
@@ -1313,7 +1334,7 @@
       <c r="F35" s="4"/>
       <c r="G35" s="49"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="3"/>
       <c r="C36" s="4"/>
@@ -1322,7 +1343,7 @@
       <c r="F36" s="4"/>
       <c r="G36" s="49"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="3"/>
       <c r="C37" s="4"/>
@@ -1331,7 +1352,7 @@
       <c r="F37" s="4"/>
       <c r="G37" s="49"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="3"/>
       <c r="C38" s="4"/>
@@ -1340,7 +1361,7 @@
       <c r="F38" s="4"/>
       <c r="G38" s="49"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="3"/>
       <c r="C39" s="4"/>
@@ -1349,7 +1370,7 @@
       <c r="F39" s="4"/>
       <c r="G39" s="49"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="3"/>
       <c r="C40" s="4"/>
@@ -1358,7 +1379,7 @@
       <c r="F40" s="4"/>
       <c r="G40" s="49"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
       <c r="B41" s="3"/>
       <c r="C41" s="4"/>
@@ -1367,7 +1388,7 @@
       <c r="F41" s="4"/>
       <c r="G41" s="49"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
       <c r="B42" s="3"/>
       <c r="C42" s="4"/>
@@ -1376,7 +1397,7 @@
       <c r="F42" s="4"/>
       <c r="G42" s="49"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
       <c r="B43" s="3"/>
       <c r="C43" s="4"/>
@@ -1385,7 +1406,7 @@
       <c r="F43" s="4"/>
       <c r="G43" s="49"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
       <c r="B44" s="3"/>
       <c r="C44" s="4"/>
@@ -1394,7 +1415,7 @@
       <c r="F44" s="4"/>
       <c r="G44" s="49"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
       <c r="B45" s="3"/>
       <c r="C45" s="4"/>
@@ -1403,7 +1424,7 @@
       <c r="F45" s="4"/>
       <c r="G45" s="49"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
       <c r="B46" s="3"/>
       <c r="C46" s="4"/>
@@ -1412,7 +1433,7 @@
       <c r="F46" s="4"/>
       <c r="G46" s="49"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
       <c r="B47" s="3"/>
       <c r="C47" s="4"/>
@@ -1421,7 +1442,7 @@
       <c r="F47" s="4"/>
       <c r="G47" s="49"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
       <c r="B48" s="3"/>
       <c r="C48" s="4"/>
@@ -1430,7 +1451,7 @@
       <c r="F48" s="4"/>
       <c r="G48" s="49"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
       <c r="B49" s="3"/>
       <c r="C49" s="4"/>
@@ -1439,7 +1460,7 @@
       <c r="F49" s="4"/>
       <c r="G49" s="49"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="5"/>
       <c r="B50" s="3"/>
       <c r="C50" s="4"/>
@@ -1448,7 +1469,7 @@
       <c r="F50" s="4"/>
       <c r="G50" s="49"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="5"/>
       <c r="B51" s="3"/>
       <c r="C51" s="4"/>
@@ -1457,7 +1478,7 @@
       <c r="F51" s="4"/>
       <c r="G51" s="49"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
       <c r="B52" s="3"/>
       <c r="C52" s="4"/>
@@ -1466,7 +1487,7 @@
       <c r="F52" s="4"/>
       <c r="G52" s="49"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="5"/>
       <c r="B53" s="3"/>
       <c r="C53" s="4"/>
@@ -1475,7 +1496,7 @@
       <c r="F53" s="4"/>
       <c r="G53" s="49"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="5"/>
       <c r="B54" s="3"/>
       <c r="C54" s="4"/>
@@ -1484,7 +1505,7 @@
       <c r="F54" s="4"/>
       <c r="G54" s="49"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="5"/>
       <c r="B55" s="3"/>
       <c r="C55" s="4"/>
@@ -1493,7 +1514,7 @@
       <c r="F55" s="4"/>
       <c r="G55" s="49"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="5"/>
       <c r="B56" s="3"/>
       <c r="C56" s="4"/>
@@ -1502,7 +1523,7 @@
       <c r="F56" s="4"/>
       <c r="G56" s="49"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="5"/>
       <c r="B57" s="3"/>
       <c r="C57" s="4"/>
@@ -1511,7 +1532,7 @@
       <c r="F57" s="4"/>
       <c r="G57" s="49"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="5"/>
       <c r="B58" s="3"/>
       <c r="C58" s="4"/>
@@ -1520,7 +1541,7 @@
       <c r="F58" s="4"/>
       <c r="G58" s="49"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="5"/>
       <c r="B59" s="3"/>
       <c r="C59" s="4"/>
@@ -1529,7 +1550,7 @@
       <c r="F59" s="4"/>
       <c r="G59" s="49"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="5"/>
       <c r="B60" s="3"/>
       <c r="C60" s="4"/>
@@ -1538,7 +1559,7 @@
       <c r="F60" s="4"/>
       <c r="G60" s="49"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="5"/>
       <c r="B61" s="3"/>
       <c r="C61" s="4"/>
@@ -1547,7 +1568,7 @@
       <c r="F61" s="4"/>
       <c r="G61" s="49"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="5"/>
       <c r="B62" s="3"/>
       <c r="C62" s="4"/>
@@ -1556,7 +1577,7 @@
       <c r="F62" s="4"/>
       <c r="G62" s="49"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="5"/>
       <c r="B63" s="3"/>
       <c r="C63" s="4"/>
@@ -1565,7 +1586,7 @@
       <c r="F63" s="4"/>
       <c r="G63" s="49"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="5"/>
       <c r="B64" s="3"/>
       <c r="C64" s="4"/>
@@ -1574,7 +1595,7 @@
       <c r="F64" s="4"/>
       <c r="G64" s="49"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="5"/>
       <c r="B65" s="3"/>
       <c r="C65" s="4"/>
@@ -1583,7 +1604,7 @@
       <c r="F65" s="4"/>
       <c r="G65" s="49"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="5"/>
       <c r="B66" s="3"/>
       <c r="C66" s="4"/>
@@ -1592,7 +1613,7 @@
       <c r="F66" s="4"/>
       <c r="G66" s="49"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="5"/>
       <c r="B67" s="3"/>
       <c r="C67" s="4"/>
@@ -1601,7 +1622,7 @@
       <c r="F67" s="4"/>
       <c r="G67" s="49"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="5"/>
       <c r="B68" s="3"/>
       <c r="C68" s="4"/>
@@ -1610,7 +1631,7 @@
       <c r="F68" s="4"/>
       <c r="G68" s="49"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="5"/>
       <c r="B69" s="3"/>
       <c r="C69" s="4"/>
@@ -1619,7 +1640,7 @@
       <c r="F69" s="4"/>
       <c r="G69" s="49"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="5"/>
       <c r="B70" s="3"/>
       <c r="C70" s="4"/>
@@ -1628,7 +1649,7 @@
       <c r="F70" s="4"/>
       <c r="G70" s="49"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="5"/>
       <c r="B71" s="3"/>
       <c r="C71" s="4"/>
@@ -1637,7 +1658,7 @@
       <c r="F71" s="4"/>
       <c r="G71" s="49"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="5"/>
       <c r="B72" s="3"/>
       <c r="C72" s="4"/>
@@ -1646,7 +1667,7 @@
       <c r="F72" s="4"/>
       <c r="G72" s="49"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="5"/>
       <c r="B73" s="3"/>
       <c r="C73" s="4"/>
@@ -1655,7 +1676,7 @@
       <c r="F73" s="4"/>
       <c r="G73" s="49"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="5"/>
       <c r="B74" s="3"/>
       <c r="C74" s="4"/>
@@ -1664,7 +1685,7 @@
       <c r="F74" s="4"/>
       <c r="G74" s="49"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="5"/>
       <c r="B75" s="3"/>
       <c r="C75" s="4"/>
@@ -1673,7 +1694,7 @@
       <c r="F75" s="4"/>
       <c r="G75" s="49"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="5"/>
       <c r="B76" s="3"/>
       <c r="C76" s="4"/>
@@ -1682,7 +1703,7 @@
       <c r="F76" s="4"/>
       <c r="G76" s="49"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="5"/>
       <c r="B77" s="3"/>
       <c r="C77" s="4"/>
@@ -1691,7 +1712,7 @@
       <c r="F77" s="4"/>
       <c r="G77" s="49"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="5"/>
       <c r="B78" s="3"/>
       <c r="C78" s="4"/>
@@ -1700,7 +1721,7 @@
       <c r="F78" s="4"/>
       <c r="G78" s="49"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="5"/>
       <c r="B79" s="3"/>
       <c r="C79" s="4"/>
@@ -1709,7 +1730,7 @@
       <c r="F79" s="4"/>
       <c r="G79" s="49"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="5"/>
       <c r="B80" s="3"/>
       <c r="C80" s="4"/>
@@ -1718,7 +1739,7 @@
       <c r="F80" s="4"/>
       <c r="G80" s="49"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="5"/>
       <c r="B81" s="3"/>
       <c r="C81" s="4"/>
@@ -1727,7 +1748,7 @@
       <c r="F81" s="4"/>
       <c r="G81" s="49"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="5"/>
       <c r="B82" s="3"/>
       <c r="C82" s="4"/>
@@ -1736,7 +1757,7 @@
       <c r="F82" s="4"/>
       <c r="G82" s="49"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="5"/>
       <c r="B83" s="3"/>
       <c r="C83" s="4"/>
@@ -1745,7 +1766,7 @@
       <c r="F83" s="4"/>
       <c r="G83" s="49"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="5"/>
       <c r="B84" s="3"/>
       <c r="C84" s="4"/>
@@ -1754,7 +1775,7 @@
       <c r="F84" s="4"/>
       <c r="G84" s="49"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="5"/>
       <c r="B85" s="3"/>
       <c r="C85" s="4"/>
@@ -1763,7 +1784,7 @@
       <c r="F85" s="4"/>
       <c r="G85" s="49"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="5"/>
       <c r="B86" s="3"/>
       <c r="C86" s="4"/>
@@ -1772,7 +1793,7 @@
       <c r="F86" s="4"/>
       <c r="G86" s="49"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="5"/>
       <c r="B87" s="3"/>
       <c r="C87" s="4"/>
@@ -1781,7 +1802,7 @@
       <c r="F87" s="4"/>
       <c r="G87" s="49"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="5"/>
       <c r="B88" s="3"/>
       <c r="C88" s="4"/>
@@ -1790,7 +1811,7 @@
       <c r="F88" s="4"/>
       <c r="G88" s="49"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="5"/>
       <c r="B89" s="3"/>
       <c r="C89" s="4"/>
@@ -1799,7 +1820,7 @@
       <c r="F89" s="4"/>
       <c r="G89" s="49"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="5"/>
       <c r="B90" s="3"/>
       <c r="C90" s="4"/>
@@ -1808,7 +1829,7 @@
       <c r="F90" s="4"/>
       <c r="G90" s="49"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="5"/>
       <c r="B91" s="3"/>
       <c r="C91" s="4"/>
@@ -1817,7 +1838,7 @@
       <c r="F91" s="4"/>
       <c r="G91" s="49"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="5"/>
       <c r="B92" s="3"/>
       <c r="C92" s="4"/>
@@ -1826,7 +1847,7 @@
       <c r="F92" s="4"/>
       <c r="G92" s="49"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="5"/>
       <c r="B93" s="3"/>
       <c r="C93" s="4"/>
@@ -1835,7 +1856,7 @@
       <c r="F93" s="4"/>
       <c r="G93" s="49"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="5"/>
       <c r="B94" s="3"/>
       <c r="C94" s="4"/>
@@ -1844,7 +1865,7 @@
       <c r="F94" s="4"/>
       <c r="G94" s="49"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="5"/>
       <c r="B95" s="3"/>
       <c r="C95" s="4"/>
@@ -1853,7 +1874,7 @@
       <c r="F95" s="4"/>
       <c r="G95" s="49"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="5"/>
       <c r="B96" s="3"/>
       <c r="C96" s="4"/>
@@ -1862,7 +1883,7 @@
       <c r="F96" s="4"/>
       <c r="G96" s="49"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="5"/>
       <c r="B97" s="3"/>
       <c r="C97" s="4"/>
@@ -1871,7 +1892,7 @@
       <c r="F97" s="4"/>
       <c r="G97" s="49"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="5"/>
       <c r="B98" s="3"/>
       <c r="C98" s="4"/>
@@ -1880,7 +1901,7 @@
       <c r="F98" s="4"/>
       <c r="G98" s="49"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="5"/>
       <c r="B99" s="3"/>
       <c r="C99" s="4"/>
@@ -1889,7 +1910,7 @@
       <c r="F99" s="4"/>
       <c r="G99" s="49"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="5"/>
       <c r="B100" s="3"/>
       <c r="C100" s="4"/>
@@ -1898,7 +1919,7 @@
       <c r="F100" s="4"/>
       <c r="G100" s="49"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="5"/>
       <c r="B101" s="3"/>
       <c r="C101" s="4"/>
@@ -1907,7 +1928,7 @@
       <c r="F101" s="4"/>
       <c r="G101" s="49"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="5"/>
       <c r="B102" s="3"/>
       <c r="C102" s="4"/>
@@ -1916,7 +1937,7 @@
       <c r="F102" s="4"/>
       <c r="G102" s="49"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="5"/>
       <c r="B103" s="3"/>
       <c r="C103" s="4"/>
@@ -1925,7 +1946,7 @@
       <c r="F103" s="4"/>
       <c r="G103" s="49"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="5"/>
       <c r="B104" s="3"/>
       <c r="C104" s="4"/>
@@ -1934,7 +1955,7 @@
       <c r="F104" s="4"/>
       <c r="G104" s="49"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="5"/>
       <c r="B105" s="3"/>
       <c r="C105" s="4"/>
@@ -1943,7 +1964,7 @@
       <c r="F105" s="4"/>
       <c r="G105" s="49"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="5"/>
       <c r="B106" s="3"/>
       <c r="C106" s="4"/>
@@ -1952,7 +1973,7 @@
       <c r="F106" s="4"/>
       <c r="G106" s="49"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="5"/>
       <c r="B107" s="3"/>
       <c r="C107" s="4"/>
@@ -1961,7 +1982,7 @@
       <c r="F107" s="4"/>
       <c r="G107" s="49"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="5"/>
       <c r="B108" s="3"/>
       <c r="C108" s="4"/>
@@ -1970,7 +1991,7 @@
       <c r="F108" s="4"/>
       <c r="G108" s="49"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="5"/>
       <c r="B109" s="3"/>
       <c r="C109" s="4"/>
@@ -1979,7 +2000,7 @@
       <c r="F109" s="4"/>
       <c r="G109" s="49"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="5"/>
       <c r="B110" s="3"/>
       <c r="C110" s="4"/>
@@ -1988,7 +2009,7 @@
       <c r="F110" s="4"/>
       <c r="G110" s="49"/>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="5"/>
       <c r="B111" s="3"/>
       <c r="C111" s="4"/>
@@ -1997,7 +2018,7 @@
       <c r="F111" s="4"/>
       <c r="G111" s="49"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="5"/>
       <c r="B112" s="3"/>
       <c r="C112" s="4"/>
@@ -2006,7 +2027,7 @@
       <c r="F112" s="4"/>
       <c r="G112" s="49"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="5"/>
       <c r="B113" s="3"/>
       <c r="C113" s="4"/>
@@ -2015,7 +2036,7 @@
       <c r="F113" s="4"/>
       <c r="G113" s="49"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="5"/>
       <c r="B114" s="3"/>
       <c r="C114" s="4"/>
@@ -2024,7 +2045,7 @@
       <c r="F114" s="4"/>
       <c r="G114" s="49"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="5"/>
       <c r="B115" s="3"/>
       <c r="C115" s="4"/>
@@ -2033,7 +2054,7 @@
       <c r="F115" s="4"/>
       <c r="G115" s="49"/>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="5"/>
       <c r="B116" s="3"/>
       <c r="C116" s="4"/>
@@ -2042,7 +2063,7 @@
       <c r="F116" s="4"/>
       <c r="G116" s="49"/>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="5"/>
       <c r="B117" s="3"/>
       <c r="C117" s="4"/>
@@ -2051,7 +2072,7 @@
       <c r="F117" s="4"/>
       <c r="G117" s="49"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="5"/>
       <c r="B118" s="3"/>
       <c r="C118" s="4"/>
@@ -2060,7 +2081,7 @@
       <c r="F118" s="4"/>
       <c r="G118" s="49"/>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="5"/>
       <c r="B119" s="3"/>
       <c r="C119" s="4"/>
@@ -2069,7 +2090,7 @@
       <c r="F119" s="4"/>
       <c r="G119" s="49"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="5"/>
       <c r="B120" s="3"/>
       <c r="C120" s="4"/>
@@ -2078,7 +2099,7 @@
       <c r="F120" s="4"/>
       <c r="G120" s="49"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="5"/>
       <c r="B121" s="3"/>
       <c r="C121" s="4"/>
@@ -2087,7 +2108,7 @@
       <c r="F121" s="4"/>
       <c r="G121" s="49"/>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="5"/>
       <c r="B122" s="3"/>
       <c r="C122" s="4"/>
@@ -2096,7 +2117,7 @@
       <c r="F122" s="4"/>
       <c r="G122" s="49"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="5"/>
       <c r="B123" s="3"/>
       <c r="C123" s="4"/>
@@ -2105,7 +2126,7 @@
       <c r="F123" s="4"/>
       <c r="G123" s="49"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="5"/>
       <c r="B124" s="3"/>
       <c r="C124" s="4"/>
@@ -2114,7 +2135,7 @@
       <c r="F124" s="4"/>
       <c r="G124" s="49"/>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="5"/>
       <c r="B125" s="3"/>
       <c r="C125" s="4"/>
@@ -2123,7 +2144,7 @@
       <c r="F125" s="4"/>
       <c r="G125" s="49"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="5"/>
       <c r="B126" s="3"/>
       <c r="C126" s="4"/>
@@ -2132,7 +2153,7 @@
       <c r="F126" s="4"/>
       <c r="G126" s="49"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="5"/>
       <c r="B127" s="3"/>
       <c r="C127" s="4"/>
@@ -2141,7 +2162,7 @@
       <c r="F127" s="4"/>
       <c r="G127" s="49"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="5"/>
       <c r="B128" s="3"/>
       <c r="C128" s="4"/>
@@ -2150,7 +2171,7 @@
       <c r="F128" s="4"/>
       <c r="G128" s="49"/>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="5"/>
       <c r="B129" s="3"/>
       <c r="C129" s="4"/>
@@ -2159,7 +2180,7 @@
       <c r="F129" s="4"/>
       <c r="G129" s="49"/>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="5"/>
       <c r="B130" s="3"/>
       <c r="C130" s="4"/>
@@ -2168,7 +2189,7 @@
       <c r="F130" s="4"/>
       <c r="G130" s="49"/>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="5"/>
       <c r="B131" s="3"/>
       <c r="C131" s="4"/>
@@ -2177,7 +2198,7 @@
       <c r="F131" s="4"/>
       <c r="G131" s="49"/>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="5"/>
       <c r="B132" s="3"/>
       <c r="C132" s="4"/>
@@ -2186,7 +2207,7 @@
       <c r="F132" s="4"/>
       <c r="G132" s="49"/>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="5"/>
       <c r="B133" s="3"/>
       <c r="C133" s="4"/>
@@ -2195,7 +2216,7 @@
       <c r="F133" s="4"/>
       <c r="G133" s="49"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="5"/>
       <c r="B134" s="3"/>
       <c r="C134" s="4"/>
@@ -2204,7 +2225,7 @@
       <c r="F134" s="4"/>
       <c r="G134" s="49"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="5"/>
       <c r="B135" s="3"/>
       <c r="C135" s="4"/>
@@ -2213,7 +2234,7 @@
       <c r="F135" s="4"/>
       <c r="G135" s="49"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="5"/>
       <c r="B136" s="3"/>
       <c r="C136" s="4"/>
@@ -2222,7 +2243,7 @@
       <c r="F136" s="4"/>
       <c r="G136" s="49"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="5"/>
       <c r="B137" s="3"/>
       <c r="C137" s="4"/>
@@ -2231,7 +2252,7 @@
       <c r="F137" s="4"/>
       <c r="G137" s="49"/>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="5"/>
       <c r="B138" s="3"/>
       <c r="C138" s="4"/>
@@ -2240,7 +2261,7 @@
       <c r="F138" s="4"/>
       <c r="G138" s="49"/>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="5"/>
       <c r="B139" s="3"/>
       <c r="C139" s="4"/>
@@ -2249,7 +2270,7 @@
       <c r="F139" s="4"/>
       <c r="G139" s="49"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="5"/>
       <c r="B140" s="3"/>
       <c r="C140" s="4"/>
@@ -2258,7 +2279,7 @@
       <c r="F140" s="4"/>
       <c r="G140" s="49"/>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="5"/>
       <c r="B141" s="3"/>
       <c r="C141" s="4"/>
@@ -2267,7 +2288,7 @@
       <c r="F141" s="4"/>
       <c r="G141" s="49"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="5"/>
       <c r="B142" s="3"/>
       <c r="C142" s="4"/>
@@ -2276,7 +2297,7 @@
       <c r="F142" s="4"/>
       <c r="G142" s="49"/>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="5"/>
       <c r="B143" s="3"/>
       <c r="C143" s="4"/>
@@ -2285,7 +2306,7 @@
       <c r="F143" s="4"/>
       <c r="G143" s="49"/>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="5"/>
       <c r="B144" s="3"/>
       <c r="C144" s="4"/>
@@ -2294,7 +2315,7 @@
       <c r="F144" s="4"/>
       <c r="G144" s="49"/>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="5"/>
       <c r="B145" s="3"/>
       <c r="C145" s="4"/>
@@ -2303,7 +2324,7 @@
       <c r="F145" s="4"/>
       <c r="G145" s="49"/>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D146" s="7">
         <f>SUM(D2:D145)</f>
         <v>0</v>
@@ -2323,22 +2344,22 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A1" s="53" t="s">
         <v>6</v>
       </c>
@@ -2349,7 +2370,7 @@
       <c r="F1" s="54"/>
       <c r="G1" s="55"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -2372,61 +2393,145 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="16"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="16"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="16"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="16"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="16"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="14">
+        <v>1234</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="15">
+        <v>45901</v>
+      </c>
+      <c r="F3" s="18">
+        <v>9</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="14">
+        <v>1234</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="15">
+        <v>45902</v>
+      </c>
+      <c r="F4" s="18">
+        <v>10</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="14">
+        <v>1234</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="15">
+        <v>45903</v>
+      </c>
+      <c r="F5" s="18">
+        <v>11</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1234</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="15">
+        <v>45904</v>
+      </c>
+      <c r="F6" s="18">
+        <v>12</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="14">
+        <v>8989</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="15">
+        <v>45901</v>
+      </c>
+      <c r="F7" s="18">
+        <v>13</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="14">
+        <v>8989</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="15">
+        <v>45902</v>
+      </c>
+      <c r="F8" s="18">
+        <v>14</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -2435,7 +2540,7 @@
       <c r="F9" s="18"/>
       <c r="G9" s="16"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="13"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
@@ -2444,7 +2549,7 @@
       <c r="F10" s="18"/>
       <c r="G10" s="16"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
@@ -2453,10 +2558,10 @@
       <c r="F11" s="18"/>
       <c r="G11" s="16"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F12" s="19">
         <f>SUM(F3:F11)</f>
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2479,20 +2584,20 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="66.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>13</v>
       </c>
@@ -2524,7 +2629,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="27"/>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
@@ -2536,7 +2641,7 @@
       <c r="I2" s="33"/>
       <c r="J2" s="34"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="27"/>
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
@@ -2548,7 +2653,7 @@
       <c r="I3" s="33"/>
       <c r="J3" s="34"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="27"/>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
@@ -2560,7 +2665,7 @@
       <c r="I4" s="33"/>
       <c r="J4" s="34"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="27"/>
       <c r="B5" s="28"/>
       <c r="C5" s="28"/>
@@ -2572,7 +2677,7 @@
       <c r="I5" s="33"/>
       <c r="J5" s="34"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="27"/>
       <c r="B6" s="28"/>
       <c r="C6" s="28"/>
@@ -2584,7 +2689,7 @@
       <c r="I6" s="33"/>
       <c r="J6" s="34"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="27"/>
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>
@@ -2596,7 +2701,7 @@
       <c r="I7" s="33"/>
       <c r="J7" s="34"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="27"/>
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
@@ -2608,7 +2713,7 @@
       <c r="I8" s="33"/>
       <c r="J8" s="34"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="27"/>
       <c r="B9" s="28"/>
       <c r="C9" s="28"/>
@@ -2620,7 +2725,7 @@
       <c r="I9" s="33"/>
       <c r="J9" s="34"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="35">
         <f>SUM(B2:B9)</f>
         <v>0</v>
@@ -2642,17 +2747,17 @@
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="56" t="s">
         <v>20</v>
       </c>
@@ -2662,7 +2767,7 @@
       <c r="E1" s="57"/>
       <c r="F1" s="57"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="36" t="s">
         <v>10</v>
       </c>
@@ -2682,7 +2787,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="44"/>
       <c r="C3" s="42"/>
@@ -2704,19 +2809,19 @@
   <sheetPr codeName="Planilha5"/>
   <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="145.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="145.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2739,367 +2844,367 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="46"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="46"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="46"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="46"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="46"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="46"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="46"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="46"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="46"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="46"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="46"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="46"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="46"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="46"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="46"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="46"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="46"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="46"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="46"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="46"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="46"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="46"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="46"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="46"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="46"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="46"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="46"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="46"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="46"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="46"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="46"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="46"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="46"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="46"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="46"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="46"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="46"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="46"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="46"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="46"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="46"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="46"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="46"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="46"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="46"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="46"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="46"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="46"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="46"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="46"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="46"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="46"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="46"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="46"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="46"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="46"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="46"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="46"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" s="46"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" s="46"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="46"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="46"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="46"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="46"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="46"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="46"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="46"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="46"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="46"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="46"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="46"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="46"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="46"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="46"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="46"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="46"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="46"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="46"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="46"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="46"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="46"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="46"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="46"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="46"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="46"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="46"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" s="46"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="46"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" s="46"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" s="46"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" s="46"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="46"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" s="46"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" s="46"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" s="46"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" s="46"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="46"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" s="46"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" s="46"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="46"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" s="46"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" s="46"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" s="46"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" s="46"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" s="46"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" s="46"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" s="46"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" s="46"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" s="46"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" s="46"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" s="46"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="46"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" s="46"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="46"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="46"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="46"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" s="46"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" s="46"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" s="46"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" s="46"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="46"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: implementa processos e exportação de receitas
</commit_message>
<xml_diff>
--- a/data/input/MODELO DE PLANILHA.xlsx
+++ b/data/input/MODELO DE PLANILHA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\OneDrive\Documentos\014 - PORTIFOLIO\conversor-planilha-txt-dominio\data\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\001 - MODELO\001 - PORTIFÓLIO\006 - projetos\conversor-planilha-txt-dominio\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B16BCEF-47C3-4559-A281-66FB7AC80823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553F0E26-A757-4C8E-9BA9-AFB7CA7494C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="843" activeTab="1" xr2:uid="{DDA27094-FF0A-42D4-8366-22E4AF05EBD8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="843" activeTab="2" xr2:uid="{DDA27094-FF0A-42D4-8366-22E4AF05EBD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Contas pagas" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t>EMPRESA</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>TARIFA - BRADESCO</t>
+  </si>
+  <si>
+    <t>CLIENTE DO GRUPO XYZ LTDA</t>
   </si>
 </sst>
 </file>
@@ -988,18 +991,18 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="77.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23" style="46" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.88671875" style="51" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" style="51" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1022,7 +1025,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
@@ -1032,7 +1035,7 @@
       <c r="G2" s="49"/>
       <c r="H2" s="47"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
@@ -1042,7 +1045,7 @@
       <c r="G3" s="49"/>
       <c r="H3" s="47"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
@@ -1052,7 +1055,7 @@
       <c r="G4" s="49"/>
       <c r="H4" s="47"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
@@ -1062,7 +1065,7 @@
       <c r="G5" s="49"/>
       <c r="H5" s="47"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
@@ -1072,7 +1075,7 @@
       <c r="G6" s="49"/>
       <c r="H6" s="47"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
@@ -1082,7 +1085,7 @@
       <c r="G7" s="49"/>
       <c r="H7" s="47"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
@@ -1091,7 +1094,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="49"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
@@ -1100,7 +1103,7 @@
       <c r="F9" s="4"/>
       <c r="G9" s="49"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
@@ -1109,7 +1112,7 @@
       <c r="F10" s="4"/>
       <c r="G10" s="49"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
@@ -1118,7 +1121,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="49"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
@@ -1127,7 +1130,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="49"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
@@ -1136,7 +1139,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="49"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
@@ -1145,7 +1148,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="49"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
@@ -1154,7 +1157,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="49"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
@@ -1163,7 +1166,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="49"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
@@ -1172,7 +1175,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="49"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
@@ -1181,7 +1184,7 @@
       <c r="F18" s="4"/>
       <c r="G18" s="49"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
@@ -1190,7 +1193,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="49"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
@@ -1199,7 +1202,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="49"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
@@ -1208,7 +1211,7 @@
       <c r="F21" s="4"/>
       <c r="G21" s="49"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
@@ -1217,7 +1220,7 @@
       <c r="F22" s="4"/>
       <c r="G22" s="49"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
@@ -1226,7 +1229,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="49"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
@@ -1235,7 +1238,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="49"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="3"/>
       <c r="C25" s="4"/>
@@ -1244,7 +1247,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="49"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="3"/>
       <c r="C26" s="4"/>
@@ -1253,7 +1256,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="49"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="3"/>
       <c r="C27" s="4"/>
@@ -1262,7 +1265,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="49"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="3"/>
       <c r="C28" s="4"/>
@@ -1271,7 +1274,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="49"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="3"/>
       <c r="C29" s="4"/>
@@ -1280,7 +1283,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="49"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="3"/>
       <c r="C30" s="4"/>
@@ -1289,7 +1292,7 @@
       <c r="F30" s="4"/>
       <c r="G30" s="49"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="3"/>
       <c r="C31" s="4"/>
@@ -1298,7 +1301,7 @@
       <c r="F31" s="4"/>
       <c r="G31" s="49"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="3"/>
       <c r="C32" s="4"/>
@@ -1307,7 +1310,7 @@
       <c r="F32" s="4"/>
       <c r="G32" s="49"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="3"/>
       <c r="C33" s="4"/>
@@ -1316,7 +1319,7 @@
       <c r="F33" s="4"/>
       <c r="G33" s="49"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="3"/>
       <c r="C34" s="4"/>
@@ -1325,7 +1328,7 @@
       <c r="F34" s="4"/>
       <c r="G34" s="49"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="3"/>
       <c r="C35" s="4"/>
@@ -1334,7 +1337,7 @@
       <c r="F35" s="4"/>
       <c r="G35" s="49"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="3"/>
       <c r="C36" s="4"/>
@@ -1343,7 +1346,7 @@
       <c r="F36" s="4"/>
       <c r="G36" s="49"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="3"/>
       <c r="C37" s="4"/>
@@ -1352,7 +1355,7 @@
       <c r="F37" s="4"/>
       <c r="G37" s="49"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="3"/>
       <c r="C38" s="4"/>
@@ -1361,7 +1364,7 @@
       <c r="F38" s="4"/>
       <c r="G38" s="49"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="3"/>
       <c r="C39" s="4"/>
@@ -1370,7 +1373,7 @@
       <c r="F39" s="4"/>
       <c r="G39" s="49"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="3"/>
       <c r="C40" s="4"/>
@@ -1379,7 +1382,7 @@
       <c r="F40" s="4"/>
       <c r="G40" s="49"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="3"/>
       <c r="C41" s="4"/>
@@ -1388,7 +1391,7 @@
       <c r="F41" s="4"/>
       <c r="G41" s="49"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="3"/>
       <c r="C42" s="4"/>
@@ -1397,7 +1400,7 @@
       <c r="F42" s="4"/>
       <c r="G42" s="49"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="3"/>
       <c r="C43" s="4"/>
@@ -1406,7 +1409,7 @@
       <c r="F43" s="4"/>
       <c r="G43" s="49"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="3"/>
       <c r="C44" s="4"/>
@@ -1415,7 +1418,7 @@
       <c r="F44" s="4"/>
       <c r="G44" s="49"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="3"/>
       <c r="C45" s="4"/>
@@ -1424,7 +1427,7 @@
       <c r="F45" s="4"/>
       <c r="G45" s="49"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="3"/>
       <c r="C46" s="4"/>
@@ -1433,7 +1436,7 @@
       <c r="F46" s="4"/>
       <c r="G46" s="49"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="3"/>
       <c r="C47" s="4"/>
@@ -1442,7 +1445,7 @@
       <c r="F47" s="4"/>
       <c r="G47" s="49"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="3"/>
       <c r="C48" s="4"/>
@@ -1451,7 +1454,7 @@
       <c r="F48" s="4"/>
       <c r="G48" s="49"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="3"/>
       <c r="C49" s="4"/>
@@ -1460,7 +1463,7 @@
       <c r="F49" s="4"/>
       <c r="G49" s="49"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="3"/>
       <c r="C50" s="4"/>
@@ -1469,7 +1472,7 @@
       <c r="F50" s="4"/>
       <c r="G50" s="49"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="3"/>
       <c r="C51" s="4"/>
@@ -1478,7 +1481,7 @@
       <c r="F51" s="4"/>
       <c r="G51" s="49"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="3"/>
       <c r="C52" s="4"/>
@@ -1487,7 +1490,7 @@
       <c r="F52" s="4"/>
       <c r="G52" s="49"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="3"/>
       <c r="C53" s="4"/>
@@ -1496,7 +1499,7 @@
       <c r="F53" s="4"/>
       <c r="G53" s="49"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="3"/>
       <c r="C54" s="4"/>
@@ -1505,7 +1508,7 @@
       <c r="F54" s="4"/>
       <c r="G54" s="49"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="3"/>
       <c r="C55" s="4"/>
@@ -1514,7 +1517,7 @@
       <c r="F55" s="4"/>
       <c r="G55" s="49"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="3"/>
       <c r="C56" s="4"/>
@@ -1523,7 +1526,7 @@
       <c r="F56" s="4"/>
       <c r="G56" s="49"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="3"/>
       <c r="C57" s="4"/>
@@ -1532,7 +1535,7 @@
       <c r="F57" s="4"/>
       <c r="G57" s="49"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="3"/>
       <c r="C58" s="4"/>
@@ -1541,7 +1544,7 @@
       <c r="F58" s="4"/>
       <c r="G58" s="49"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
       <c r="B59" s="3"/>
       <c r="C59" s="4"/>
@@ -1550,7 +1553,7 @@
       <c r="F59" s="4"/>
       <c r="G59" s="49"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="B60" s="3"/>
       <c r="C60" s="4"/>
@@ -1559,7 +1562,7 @@
       <c r="F60" s="4"/>
       <c r="G60" s="49"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="3"/>
       <c r="C61" s="4"/>
@@ -1568,7 +1571,7 @@
       <c r="F61" s="4"/>
       <c r="G61" s="49"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="3"/>
       <c r="C62" s="4"/>
@@ -1577,7 +1580,7 @@
       <c r="F62" s="4"/>
       <c r="G62" s="49"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="3"/>
       <c r="C63" s="4"/>
@@ -1586,7 +1589,7 @@
       <c r="F63" s="4"/>
       <c r="G63" s="49"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="B64" s="3"/>
       <c r="C64" s="4"/>
@@ -1595,7 +1598,7 @@
       <c r="F64" s="4"/>
       <c r="G64" s="49"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="3"/>
       <c r="C65" s="4"/>
@@ -1604,7 +1607,7 @@
       <c r="F65" s="4"/>
       <c r="G65" s="49"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="B66" s="3"/>
       <c r="C66" s="4"/>
@@ -1613,7 +1616,7 @@
       <c r="F66" s="4"/>
       <c r="G66" s="49"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="3"/>
       <c r="C67" s="4"/>
@@ -1622,7 +1625,7 @@
       <c r="F67" s="4"/>
       <c r="G67" s="49"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="B68" s="3"/>
       <c r="C68" s="4"/>
@@ -1631,7 +1634,7 @@
       <c r="F68" s="4"/>
       <c r="G68" s="49"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="3"/>
       <c r="C69" s="4"/>
@@ -1640,7 +1643,7 @@
       <c r="F69" s="4"/>
       <c r="G69" s="49"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="3"/>
       <c r="C70" s="4"/>
@@ -1649,7 +1652,7 @@
       <c r="F70" s="4"/>
       <c r="G70" s="49"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="3"/>
       <c r="C71" s="4"/>
@@ -1658,7 +1661,7 @@
       <c r="F71" s="4"/>
       <c r="G71" s="49"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="3"/>
       <c r="C72" s="4"/>
@@ -1667,7 +1670,7 @@
       <c r="F72" s="4"/>
       <c r="G72" s="49"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="3"/>
       <c r="C73" s="4"/>
@@ -1676,7 +1679,7 @@
       <c r="F73" s="4"/>
       <c r="G73" s="49"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="3"/>
       <c r="C74" s="4"/>
@@ -1685,7 +1688,7 @@
       <c r="F74" s="4"/>
       <c r="G74" s="49"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="3"/>
       <c r="C75" s="4"/>
@@ -1694,7 +1697,7 @@
       <c r="F75" s="4"/>
       <c r="G75" s="49"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
       <c r="B76" s="3"/>
       <c r="C76" s="4"/>
@@ -1703,7 +1706,7 @@
       <c r="F76" s="4"/>
       <c r="G76" s="49"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="B77" s="3"/>
       <c r="C77" s="4"/>
@@ -1712,7 +1715,7 @@
       <c r="F77" s="4"/>
       <c r="G77" s="49"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="B78" s="3"/>
       <c r="C78" s="4"/>
@@ -1721,7 +1724,7 @@
       <c r="F78" s="4"/>
       <c r="G78" s="49"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="B79" s="3"/>
       <c r="C79" s="4"/>
@@ -1730,7 +1733,7 @@
       <c r="F79" s="4"/>
       <c r="G79" s="49"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="B80" s="3"/>
       <c r="C80" s="4"/>
@@ -1739,7 +1742,7 @@
       <c r="F80" s="4"/>
       <c r="G80" s="49"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="B81" s="3"/>
       <c r="C81" s="4"/>
@@ -1748,7 +1751,7 @@
       <c r="F81" s="4"/>
       <c r="G81" s="49"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
       <c r="B82" s="3"/>
       <c r="C82" s="4"/>
@@ -1757,7 +1760,7 @@
       <c r="F82" s="4"/>
       <c r="G82" s="49"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
       <c r="B83" s="3"/>
       <c r="C83" s="4"/>
@@ -1766,7 +1769,7 @@
       <c r="F83" s="4"/>
       <c r="G83" s="49"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
       <c r="B84" s="3"/>
       <c r="C84" s="4"/>
@@ -1775,7 +1778,7 @@
       <c r="F84" s="4"/>
       <c r="G84" s="49"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
       <c r="B85" s="3"/>
       <c r="C85" s="4"/>
@@ -1784,7 +1787,7 @@
       <c r="F85" s="4"/>
       <c r="G85" s="49"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
       <c r="B86" s="3"/>
       <c r="C86" s="4"/>
@@ -1793,7 +1796,7 @@
       <c r="F86" s="4"/>
       <c r="G86" s="49"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
       <c r="B87" s="3"/>
       <c r="C87" s="4"/>
@@ -1802,7 +1805,7 @@
       <c r="F87" s="4"/>
       <c r="G87" s="49"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
       <c r="B88" s="3"/>
       <c r="C88" s="4"/>
@@ -1811,7 +1814,7 @@
       <c r="F88" s="4"/>
       <c r="G88" s="49"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="B89" s="3"/>
       <c r="C89" s="4"/>
@@ -1820,7 +1823,7 @@
       <c r="F89" s="4"/>
       <c r="G89" s="49"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="5"/>
       <c r="B90" s="3"/>
       <c r="C90" s="4"/>
@@ -1829,7 +1832,7 @@
       <c r="F90" s="4"/>
       <c r="G90" s="49"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
       <c r="B91" s="3"/>
       <c r="C91" s="4"/>
@@ -1838,7 +1841,7 @@
       <c r="F91" s="4"/>
       <c r="G91" s="49"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="5"/>
       <c r="B92" s="3"/>
       <c r="C92" s="4"/>
@@ -1847,7 +1850,7 @@
       <c r="F92" s="4"/>
       <c r="G92" s="49"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="5"/>
       <c r="B93" s="3"/>
       <c r="C93" s="4"/>
@@ -1856,7 +1859,7 @@
       <c r="F93" s="4"/>
       <c r="G93" s="49"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="5"/>
       <c r="B94" s="3"/>
       <c r="C94" s="4"/>
@@ -1865,7 +1868,7 @@
       <c r="F94" s="4"/>
       <c r="G94" s="49"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
       <c r="B95" s="3"/>
       <c r="C95" s="4"/>
@@ -1874,7 +1877,7 @@
       <c r="F95" s="4"/>
       <c r="G95" s="49"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="5"/>
       <c r="B96" s="3"/>
       <c r="C96" s="4"/>
@@ -1883,7 +1886,7 @@
       <c r="F96" s="4"/>
       <c r="G96" s="49"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="5"/>
       <c r="B97" s="3"/>
       <c r="C97" s="4"/>
@@ -1892,7 +1895,7 @@
       <c r="F97" s="4"/>
       <c r="G97" s="49"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="5"/>
       <c r="B98" s="3"/>
       <c r="C98" s="4"/>
@@ -1901,7 +1904,7 @@
       <c r="F98" s="4"/>
       <c r="G98" s="49"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
       <c r="B99" s="3"/>
       <c r="C99" s="4"/>
@@ -1910,7 +1913,7 @@
       <c r="F99" s="4"/>
       <c r="G99" s="49"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="5"/>
       <c r="B100" s="3"/>
       <c r="C100" s="4"/>
@@ -1919,7 +1922,7 @@
       <c r="F100" s="4"/>
       <c r="G100" s="49"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
       <c r="B101" s="3"/>
       <c r="C101" s="4"/>
@@ -1928,7 +1931,7 @@
       <c r="F101" s="4"/>
       <c r="G101" s="49"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="5"/>
       <c r="B102" s="3"/>
       <c r="C102" s="4"/>
@@ -1937,7 +1940,7 @@
       <c r="F102" s="4"/>
       <c r="G102" s="49"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="5"/>
       <c r="B103" s="3"/>
       <c r="C103" s="4"/>
@@ -1946,7 +1949,7 @@
       <c r="F103" s="4"/>
       <c r="G103" s="49"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
       <c r="B104" s="3"/>
       <c r="C104" s="4"/>
@@ -1955,7 +1958,7 @@
       <c r="F104" s="4"/>
       <c r="G104" s="49"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="5"/>
       <c r="B105" s="3"/>
       <c r="C105" s="4"/>
@@ -1964,7 +1967,7 @@
       <c r="F105" s="4"/>
       <c r="G105" s="49"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="5"/>
       <c r="B106" s="3"/>
       <c r="C106" s="4"/>
@@ -1973,7 +1976,7 @@
       <c r="F106" s="4"/>
       <c r="G106" s="49"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="5"/>
       <c r="B107" s="3"/>
       <c r="C107" s="4"/>
@@ -1982,7 +1985,7 @@
       <c r="F107" s="4"/>
       <c r="G107" s="49"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="5"/>
       <c r="B108" s="3"/>
       <c r="C108" s="4"/>
@@ -1991,7 +1994,7 @@
       <c r="F108" s="4"/>
       <c r="G108" s="49"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="5"/>
       <c r="B109" s="3"/>
       <c r="C109" s="4"/>
@@ -2000,7 +2003,7 @@
       <c r="F109" s="4"/>
       <c r="G109" s="49"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="5"/>
       <c r="B110" s="3"/>
       <c r="C110" s="4"/>
@@ -2009,7 +2012,7 @@
       <c r="F110" s="4"/>
       <c r="G110" s="49"/>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
       <c r="B111" s="3"/>
       <c r="C111" s="4"/>
@@ -2018,7 +2021,7 @@
       <c r="F111" s="4"/>
       <c r="G111" s="49"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="5"/>
       <c r="B112" s="3"/>
       <c r="C112" s="4"/>
@@ -2027,7 +2030,7 @@
       <c r="F112" s="4"/>
       <c r="G112" s="49"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="5"/>
       <c r="B113" s="3"/>
       <c r="C113" s="4"/>
@@ -2036,7 +2039,7 @@
       <c r="F113" s="4"/>
       <c r="G113" s="49"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="5"/>
       <c r="B114" s="3"/>
       <c r="C114" s="4"/>
@@ -2045,7 +2048,7 @@
       <c r="F114" s="4"/>
       <c r="G114" s="49"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="5"/>
       <c r="B115" s="3"/>
       <c r="C115" s="4"/>
@@ -2054,7 +2057,7 @@
       <c r="F115" s="4"/>
       <c r="G115" s="49"/>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="5"/>
       <c r="B116" s="3"/>
       <c r="C116" s="4"/>
@@ -2063,7 +2066,7 @@
       <c r="F116" s="4"/>
       <c r="G116" s="49"/>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="5"/>
       <c r="B117" s="3"/>
       <c r="C117" s="4"/>
@@ -2072,7 +2075,7 @@
       <c r="F117" s="4"/>
       <c r="G117" s="49"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="5"/>
       <c r="B118" s="3"/>
       <c r="C118" s="4"/>
@@ -2081,7 +2084,7 @@
       <c r="F118" s="4"/>
       <c r="G118" s="49"/>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="5"/>
       <c r="B119" s="3"/>
       <c r="C119" s="4"/>
@@ -2090,7 +2093,7 @@
       <c r="F119" s="4"/>
       <c r="G119" s="49"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="5"/>
       <c r="B120" s="3"/>
       <c r="C120" s="4"/>
@@ -2099,7 +2102,7 @@
       <c r="F120" s="4"/>
       <c r="G120" s="49"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="5"/>
       <c r="B121" s="3"/>
       <c r="C121" s="4"/>
@@ -2108,7 +2111,7 @@
       <c r="F121" s="4"/>
       <c r="G121" s="49"/>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="5"/>
       <c r="B122" s="3"/>
       <c r="C122" s="4"/>
@@ -2117,7 +2120,7 @@
       <c r="F122" s="4"/>
       <c r="G122" s="49"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="5"/>
       <c r="B123" s="3"/>
       <c r="C123" s="4"/>
@@ -2126,7 +2129,7 @@
       <c r="F123" s="4"/>
       <c r="G123" s="49"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="5"/>
       <c r="B124" s="3"/>
       <c r="C124" s="4"/>
@@ -2135,7 +2138,7 @@
       <c r="F124" s="4"/>
       <c r="G124" s="49"/>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="5"/>
       <c r="B125" s="3"/>
       <c r="C125" s="4"/>
@@ -2144,7 +2147,7 @@
       <c r="F125" s="4"/>
       <c r="G125" s="49"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="5"/>
       <c r="B126" s="3"/>
       <c r="C126" s="4"/>
@@ -2153,7 +2156,7 @@
       <c r="F126" s="4"/>
       <c r="G126" s="49"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="5"/>
       <c r="B127" s="3"/>
       <c r="C127" s="4"/>
@@ -2162,7 +2165,7 @@
       <c r="F127" s="4"/>
       <c r="G127" s="49"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="5"/>
       <c r="B128" s="3"/>
       <c r="C128" s="4"/>
@@ -2171,7 +2174,7 @@
       <c r="F128" s="4"/>
       <c r="G128" s="49"/>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="5"/>
       <c r="B129" s="3"/>
       <c r="C129" s="4"/>
@@ -2180,7 +2183,7 @@
       <c r="F129" s="4"/>
       <c r="G129" s="49"/>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="5"/>
       <c r="B130" s="3"/>
       <c r="C130" s="4"/>
@@ -2189,7 +2192,7 @@
       <c r="F130" s="4"/>
       <c r="G130" s="49"/>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="5"/>
       <c r="B131" s="3"/>
       <c r="C131" s="4"/>
@@ -2198,7 +2201,7 @@
       <c r="F131" s="4"/>
       <c r="G131" s="49"/>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="5"/>
       <c r="B132" s="3"/>
       <c r="C132" s="4"/>
@@ -2207,7 +2210,7 @@
       <c r="F132" s="4"/>
       <c r="G132" s="49"/>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="5"/>
       <c r="B133" s="3"/>
       <c r="C133" s="4"/>
@@ -2216,7 +2219,7 @@
       <c r="F133" s="4"/>
       <c r="G133" s="49"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="5"/>
       <c r="B134" s="3"/>
       <c r="C134" s="4"/>
@@ -2225,7 +2228,7 @@
       <c r="F134" s="4"/>
       <c r="G134" s="49"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="5"/>
       <c r="B135" s="3"/>
       <c r="C135" s="4"/>
@@ -2234,7 +2237,7 @@
       <c r="F135" s="4"/>
       <c r="G135" s="49"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="5"/>
       <c r="B136" s="3"/>
       <c r="C136" s="4"/>
@@ -2243,7 +2246,7 @@
       <c r="F136" s="4"/>
       <c r="G136" s="49"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="5"/>
       <c r="B137" s="3"/>
       <c r="C137" s="4"/>
@@ -2252,7 +2255,7 @@
       <c r="F137" s="4"/>
       <c r="G137" s="49"/>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="5"/>
       <c r="B138" s="3"/>
       <c r="C138" s="4"/>
@@ -2261,7 +2264,7 @@
       <c r="F138" s="4"/>
       <c r="G138" s="49"/>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="5"/>
       <c r="B139" s="3"/>
       <c r="C139" s="4"/>
@@ -2270,7 +2273,7 @@
       <c r="F139" s="4"/>
       <c r="G139" s="49"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="5"/>
       <c r="B140" s="3"/>
       <c r="C140" s="4"/>
@@ -2279,7 +2282,7 @@
       <c r="F140" s="4"/>
       <c r="G140" s="49"/>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="5"/>
       <c r="B141" s="3"/>
       <c r="C141" s="4"/>
@@ -2288,7 +2291,7 @@
       <c r="F141" s="4"/>
       <c r="G141" s="49"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="5"/>
       <c r="B142" s="3"/>
       <c r="C142" s="4"/>
@@ -2297,7 +2300,7 @@
       <c r="F142" s="4"/>
       <c r="G142" s="49"/>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="5"/>
       <c r="B143" s="3"/>
       <c r="C143" s="4"/>
@@ -2306,7 +2309,7 @@
       <c r="F143" s="4"/>
       <c r="G143" s="49"/>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="5"/>
       <c r="B144" s="3"/>
       <c r="C144" s="4"/>
@@ -2315,7 +2318,7 @@
       <c r="F144" s="4"/>
       <c r="G144" s="49"/>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="5"/>
       <c r="B145" s="3"/>
       <c r="C145" s="4"/>
@@ -2324,7 +2327,7 @@
       <c r="F145" s="4"/>
       <c r="G145" s="49"/>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D146" s="7">
         <f>SUM(D2:D145)</f>
         <v>0</v>
@@ -2344,22 +2347,22 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.600000000000001" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A1" s="53" t="s">
         <v>6</v>
       </c>
@@ -2370,7 +2373,7 @@
       <c r="F1" s="54"/>
       <c r="G1" s="55"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -2393,7 +2396,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>30</v>
       </c>
@@ -2416,7 +2419,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>30</v>
       </c>
@@ -2439,7 +2442,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>30</v>
       </c>
@@ -2462,7 +2465,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>30</v>
       </c>
@@ -2485,7 +2488,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>30</v>
       </c>
@@ -2508,7 +2511,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>30</v>
       </c>
@@ -2531,7 +2534,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -2540,7 +2543,7 @@
       <c r="F9" s="18"/>
       <c r="G9" s="16"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
@@ -2549,7 +2552,7 @@
       <c r="F10" s="18"/>
       <c r="G10" s="16"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
@@ -2558,7 +2561,7 @@
       <c r="F11" s="18"/>
       <c r="G11" s="16"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F12" s="19">
         <f>SUM(F3:F11)</f>
         <v>69</v>
@@ -2580,24 +2583,24 @@
   </sheetPr>
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="66.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>13</v>
       </c>
@@ -2629,55 +2632,103 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="27"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="30"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="27">
+        <v>45902</v>
+      </c>
+      <c r="B2" s="28">
+        <v>150000</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>37</v>
+      </c>
       <c r="F2" s="48"/>
       <c r="G2" s="32"/>
       <c r="H2" s="32"/>
-      <c r="I2" s="33"/>
+      <c r="I2" s="33">
+        <v>1</v>
+      </c>
       <c r="J2" s="34"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="27"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="30"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="27">
+        <v>45930</v>
+      </c>
+      <c r="B3" s="28">
+        <v>50000</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>37</v>
+      </c>
       <c r="F3" s="48"/>
       <c r="G3" s="32"/>
       <c r="H3" s="32"/>
-      <c r="I3" s="33"/>
+      <c r="I3" s="33">
+        <v>2</v>
+      </c>
       <c r="J3" s="34"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="27"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="27">
+        <v>45901</v>
+      </c>
+      <c r="B4" s="28">
+        <v>350000</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>37</v>
+      </c>
       <c r="F4" s="31"/>
       <c r="G4" s="32"/>
       <c r="H4" s="32"/>
-      <c r="I4" s="33"/>
+      <c r="I4" s="33">
+        <v>3</v>
+      </c>
       <c r="J4" s="34"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="27"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="30"/>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="27">
+        <v>45910</v>
+      </c>
+      <c r="B5" s="28">
+        <v>50000</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>37</v>
+      </c>
       <c r="F5" s="31"/>
       <c r="G5" s="32"/>
       <c r="H5" s="32"/>
-      <c r="I5" s="33"/>
+      <c r="I5" s="33">
+        <v>4</v>
+      </c>
       <c r="J5" s="34"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="27"/>
       <c r="B6" s="28"/>
       <c r="C6" s="28"/>
@@ -2689,7 +2740,7 @@
       <c r="I6" s="33"/>
       <c r="J6" s="34"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="27"/>
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>
@@ -2701,7 +2752,7 @@
       <c r="I7" s="33"/>
       <c r="J7" s="34"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="27"/>
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
@@ -2713,7 +2764,7 @@
       <c r="I8" s="33"/>
       <c r="J8" s="34"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="27"/>
       <c r="B9" s="28"/>
       <c r="C9" s="28"/>
@@ -2725,10 +2776,10 @@
       <c r="I9" s="33"/>
       <c r="J9" s="34"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="35">
         <f>SUM(B2:B9)</f>
-        <v>0</v>
+        <v>600000</v>
       </c>
       <c r="C10" s="45"/>
     </row>
@@ -2747,17 +2798,17 @@
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="56" t="s">
         <v>20</v>
       </c>
@@ -2767,7 +2818,7 @@
       <c r="E1" s="57"/>
       <c r="F1" s="57"/>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="36" t="s">
         <v>10</v>
       </c>
@@ -2787,7 +2838,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="41"/>
       <c r="B3" s="44"/>
       <c r="C3" s="42"/>
@@ -2811,17 +2862,17 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="145.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="145.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2844,367 +2895,367 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="46"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="46"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="46"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="46"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="46"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="46"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="46"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="46"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="46"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="46"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="46"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="46"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="46"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="46"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="46"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="46"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="46"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="46"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="46"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="46"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="46"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="46"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="46"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="46"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="46"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="46"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="46"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="46"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="46"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="46"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="46"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="46"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="46"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="46"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="46"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="46"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="46"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="46"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="46"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="46"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="46"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="46"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="46"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="46"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="46"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="46"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="46"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="46"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="46"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="46"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="46"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="46"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="46"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="46"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="46"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="46"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="46"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="46"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="46"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="46"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="46"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="46"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="46"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="46"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="46"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="46"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="46"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="46"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="46"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="46"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="46"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="46"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="46"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="46"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="46"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="46"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="46"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="46"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="46"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="46"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="46"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="46"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="46"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="46"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="46"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="46"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="46"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="46"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="46"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="46"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="46"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="46"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="46"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="46"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="46"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="46"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="46"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="46"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="46"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="46"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="46"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="46"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="46"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="46"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="46"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="46"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="46"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="46"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="46"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="46"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="46"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="46"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="46"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="46"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="46"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="46"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="46"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="46"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="46"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="46"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="46"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementação da leitura e lançamentos da apropriações
</commit_message>
<xml_diff>
--- a/data/input/MODELO DE PLANILHA.xlsx
+++ b/data/input/MODELO DE PLANILHA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\001 - MODELO\001 - PORTIFÓLIO\006 - projetos\conversor-planilha-txt-dominio\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553F0E26-A757-4C8E-9BA9-AFB7CA7494C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1643521A-7557-42A8-AB2C-57D7BCF225F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="843" activeTab="2" xr2:uid="{DDA27094-FF0A-42D4-8366-22E4AF05EBD8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="843" activeTab="4" xr2:uid="{DDA27094-FF0A-42D4-8366-22E4AF05EBD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Contas pagas" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="42">
   <si>
     <t>EMPRESA</t>
   </si>
@@ -158,6 +158,18 @@
   </si>
   <si>
     <t>CLIENTE DO GRUPO XYZ LTDA</t>
+  </si>
+  <si>
+    <t>APROP. CONF NF 23 FORNECEDOR DO GRUPO XYZ</t>
+  </si>
+  <si>
+    <t>TRANSF. ENTRE CONTAS</t>
+  </si>
+  <si>
+    <t>APLICAÇÃO</t>
+  </si>
+  <si>
+    <t>RESGATE DE APLICAÇÃO</t>
   </si>
 </sst>
 </file>
@@ -2583,8 +2595,8 @@
   </sheetPr>
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2860,7 +2872,9 @@
   <sheetPr codeName="Planilha5"/>
   <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2896,19 +2910,104 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
+      <c r="A2" s="46">
+        <v>45902</v>
+      </c>
+      <c r="B2">
+        <v>40085</v>
+      </c>
+      <c r="C2">
+        <v>20135</v>
+      </c>
+      <c r="D2" s="47">
+        <v>50125</v>
+      </c>
+      <c r="E2">
+        <v>253</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
+      <c r="A3" s="46">
+        <v>45930</v>
+      </c>
+      <c r="B3">
+        <v>10008</v>
+      </c>
+      <c r="C3">
+        <v>10017</v>
+      </c>
+      <c r="D3" s="47">
+        <v>23585.23</v>
+      </c>
+      <c r="E3">
+        <v>253</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
+      <c r="A4" s="46">
+        <v>45905</v>
+      </c>
+      <c r="B4">
+        <v>40085</v>
+      </c>
+      <c r="C4">
+        <v>20133</v>
+      </c>
+      <c r="D4" s="47">
+        <v>5412.25</v>
+      </c>
+      <c r="E4">
+        <v>253</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
+      <c r="A5" s="46">
+        <v>45915</v>
+      </c>
+      <c r="B5">
+        <v>10017</v>
+      </c>
+      <c r="C5">
+        <v>10008</v>
+      </c>
+      <c r="D5" s="47">
+        <v>23.24</v>
+      </c>
+      <c r="E5">
+        <v>253</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
+      <c r="A6" s="46">
+        <v>45920</v>
+      </c>
+      <c r="B6">
+        <v>10009</v>
+      </c>
+      <c r="C6">
+        <v>10008</v>
+      </c>
+      <c r="D6" s="47">
+        <v>21544.22</v>
+      </c>
+      <c r="E6">
+        <v>253</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="46"/>

</xml_diff>